<commit_message>
Updates import API to process multiple sheets and removes dependance on node-xlsx library (prefer just exceljs)
</commit_message>
<xml_diff>
--- a/bctw-api/src/import/test.xlsx
+++ b/bctw-api/src/import/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="21300" yWindow="4485" windowWidth="26640" windowHeight="14730" activeTab="1"/>
+    <workbookView xWindow="-26550" yWindow="2610" windowWidth="24765" windowHeight="14430"/>
   </bookViews>
   <sheets>
     <sheet sheetId="2" name="Device Metadata" state="visible" r:id="rId4"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="177">
   <si>
     <t>Wildlife Health ID</t>
   </si>
@@ -119,13 +119,13 @@
     <t>Frequency</t>
   </si>
   <si>
-    <t>Frequency Units</t>
+    <t>Frequency Unit</t>
   </si>
   <si>
     <t>Fix Interval</t>
   </si>
   <si>
-    <t>Fix Interval Units</t>
+    <t>Fix Interval Rate</t>
   </si>
   <si>
     <t>Satellite Network</t>
@@ -149,16 +149,16 @@
     <t>Malfunction Date</t>
   </si>
   <si>
-    <t>Malfunction Comments</t>
-  </si>
-  <si>
-    <t>Malfunctioning Device Type</t>
+    <t>Malfunction Comment</t>
+  </si>
+  <si>
+    <t>Device Malfunction Type</t>
   </si>
   <si>
     <t>Device Retrieval Date</t>
   </si>
   <si>
-    <t>Device Retrieval Comments</t>
+    <t>Device Retrieval Comment</t>
   </si>
   <si>
     <t>Animal Mortality Date</t>
@@ -167,7 +167,7 @@
     <t>Suspected Mortality Cause</t>
   </si>
   <si>
-    <t>Mortality Comments</t>
+    <t>Mortality Comment</t>
   </si>
   <si>
     <t>Species Values</t>
@@ -194,9 +194,18 @@
     <t>Device Type Values</t>
   </si>
   <si>
+    <t>Frequency Unit Values</t>
+  </si>
+  <si>
     <t>Satellite Network Values</t>
   </si>
   <si>
+    <t>Device Malfunction Type Values</t>
+  </si>
+  <si>
+    <t>Suspected Mortality Cause Values</t>
+  </si>
+  <si>
     <t>Caribou</t>
   </si>
   <si>
@@ -221,9 +230,18 @@
     <t>GPS</t>
   </si>
   <si>
+    <t>Hz</t>
+  </si>
+  <si>
     <t>Argos</t>
   </si>
   <si>
+    <t>Battery</t>
+  </si>
+  <si>
+    <t>Accident Avalanche</t>
+  </si>
+  <si>
     <t>Grey Wolf</t>
   </si>
   <si>
@@ -248,9 +266,18 @@
     <t>GPS/GSM</t>
   </si>
   <si>
+    <t>KHz</t>
+  </si>
+  <si>
     <t>Globalstar</t>
   </si>
   <si>
+    <t>Drop-off</t>
+  </si>
+  <si>
+    <t>Accident Capture</t>
+  </si>
+  <si>
     <t>Grizzly Bear</t>
   </si>
   <si>
@@ -275,9 +302,15 @@
     <t>SAT/GPS</t>
   </si>
   <si>
+    <t>MHz</t>
+  </si>
+  <si>
     <t>Iridium</t>
   </si>
   <si>
+    <t>Accident Collision</t>
+  </si>
+  <si>
     <t>Moose</t>
   </si>
   <si>
@@ -296,6 +329,12 @@
     <t>VHF</t>
   </si>
   <si>
+    <t>GPS &amp; VHF</t>
+  </si>
+  <si>
+    <t>Accident Natural</t>
+  </si>
+  <si>
     <t>Carcross</t>
   </si>
   <si>
@@ -305,6 +344,12 @@
     <t>Telonics</t>
   </si>
   <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Defense Life Property</t>
+  </si>
+  <si>
     <t>Central Rockies</t>
   </si>
   <si>
@@ -314,46 +359,79 @@
     <t>Vectronic</t>
   </si>
   <si>
+    <t>Health Related</t>
+  </si>
+  <si>
     <t>Central Selkirks</t>
   </si>
   <si>
     <t>Skeena</t>
   </si>
   <si>
+    <t>Hunting Aboriginal</t>
+  </si>
+  <si>
     <t>Charlotte Alplands</t>
   </si>
   <si>
     <t>Thompson</t>
   </si>
   <si>
+    <t>Hunting Licenced</t>
+  </si>
+  <si>
     <t>Chase</t>
   </si>
   <si>
     <t>Vancouver Island</t>
   </si>
   <si>
+    <t>Hunting Unlicenced</t>
+  </si>
+  <si>
     <t>Chinchaga</t>
   </si>
   <si>
+    <t>Natural</t>
+  </si>
+  <si>
     <t>Columbia North</t>
   </si>
   <si>
     <t>Columbia South</t>
   </si>
   <si>
+    <t>Poisioning</t>
+  </si>
+  <si>
     <t>Edziza</t>
   </si>
   <si>
+    <t>Predation Location</t>
+  </si>
+  <si>
     <t>Finlay</t>
   </si>
   <si>
+    <t>Predation No Location</t>
+  </si>
+  <si>
     <t>Frisby-Boulder</t>
   </si>
   <si>
+    <t>Predation Probable</t>
+  </si>
+  <si>
     <t>Frog</t>
   </si>
   <si>
+    <t>Removal</t>
+  </si>
+  <si>
     <t>Gataga</t>
+  </si>
+  <si>
+    <t>Trapping</t>
   </si>
   <si>
     <t>George Mtn</t>
@@ -571,12 +649,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -921,172 +1002,177 @@
   <dimension ref="A1:AY1"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="91" zoomScaleNormal="91">
-      <selection activeCell="AA16" sqref="AA16"/>
+      <selection activeCell="AK4" sqref="AK4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" defaultColWidth="10.7109375"/>
   <cols>
     <col min="1" max="18" width="10.7109375" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="10.7109375" style="2" customWidth="1"/>
+    <col min="19" max="43" width="10.7109375" style="2" customWidth="1"/>
+    <col min="44" max="44" width="12.140625" style="3" customWidth="1"/>
+    <col min="45" max="45" width="11.7109375" style="3" customWidth="1"/>
+    <col min="46" max="46" width="11.85546875" style="3" customWidth="1"/>
+    <col min="47" max="51" width="10.7109375" style="3" customWidth="1"/>
+    <col min="52" max="16384" width="10.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="49.9" customHeight="1" spans="1:51" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" ht="49.9" customHeight="1" spans="1:51" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="S1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="U1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="V1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="W1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="X1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Y1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="Z1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AA1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AB1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AC1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="8" t="s">
+      <c r="AD1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="8" t="s">
+      <c r="AE1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="8" t="s">
+      <c r="AF1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="8" t="s">
+      <c r="AG1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="8" t="s">
+      <c r="AH1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="8" t="s">
+      <c r="AI1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="8" t="s">
+      <c r="AJ1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="8" t="s">
+      <c r="AK1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="8" t="s">
+      <c r="AL1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="8" t="s">
+      <c r="AM1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="8" t="s">
+      <c r="AN1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="8" t="s">
+      <c r="AO1" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="8" t="s">
+      <c r="AP1" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="8" t="s">
+      <c r="AQ1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="8" t="s">
+      <c r="AR1" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="8" t="s">
+      <c r="AS1" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="8" t="s">
+      <c r="AT1" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="9" t="s">
+      <c r="AU1" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="9" t="s">
+      <c r="AV1" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="10" t="s">
+      <c r="AW1" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="10" t="s">
+      <c r="AX1" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="10" t="s">
+      <c r="AY1" s="11" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="9">
+  <dataValidations count="12">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Selection" error="Please use the drop down to select a valid value" sqref="AD2:AD9999">
       <formula1>Validation!F2:F4</formula1>
     </dataValidation>
@@ -1096,8 +1182,17 @@
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Selection" error="Please use the drop down to select a valid value" sqref="AG2:AG9999">
       <formula1>Validation!H2:H5</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Selection" error="Please use the drop down to select a valid value" sqref="AI2:AI9999">
+      <formula1>Validation!I2:I4</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Selection" error="Please use the drop down to select a valid value" sqref="AL2:AL9999">
-      <formula1>Validation!I2:I4</formula1>
+      <formula1>Validation!J2:J4</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Selection" error="Please use the drop down to select a valid value" sqref="AT2:AT9999">
+      <formula1>Validation!K2:K8</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Selection" error="Please use the drop down to select a valid value" sqref="AX2:AX9999">
+      <formula1>Validation!L2:L19</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Selection" error="Please use the drop down to select a valid value" sqref="C2:C9999">
       <formula1>Validation!A2:A5</formula1>
@@ -1122,425 +1217,518 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I56"/>
+  <dimension ref="A1:L56"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="12" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="G2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="H2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="I2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="J2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" t="s">
+        <v>73</v>
+      </c>
+      <c r="L2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H3" t="s">
+        <v>82</v>
+      </c>
+      <c r="I3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K3" t="s">
+        <v>85</v>
+      </c>
+      <c r="L3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H4" t="s">
+        <v>94</v>
+      </c>
+      <c r="I4" t="s">
+        <v>95</v>
+      </c>
+      <c r="J4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K4" t="s">
         <v>70</v>
       </c>
-      <c r="C3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G3" t="s">
-        <v>75</v>
-      </c>
-      <c r="H3" t="s">
-        <v>76</v>
-      </c>
-      <c r="I3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F4" t="s">
-        <v>83</v>
-      </c>
-      <c r="G4" t="s">
-        <v>84</v>
-      </c>
-      <c r="H4" t="s">
-        <v>85</v>
-      </c>
-      <c r="I4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="C5" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="E5" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="G5" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="H5" t="s">
+        <v>103</v>
+      </c>
+      <c r="K5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E6" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C6" t="s">
-        <v>94</v>
-      </c>
-      <c r="E6" t="s">
-        <v>83</v>
-      </c>
       <c r="G6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="K6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="C7" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="G7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="K7" t="s">
+        <v>92</v>
+      </c>
+      <c r="L7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="C8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="K8" t="s">
+        <v>103</v>
+      </c>
+      <c r="L8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="C9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="L9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="C10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="L10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="L11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="L12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="L13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="L14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="L15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+      <c r="L16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="L17" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="L18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>113</v>
+        <v>139</v>
+      </c>
+      <c r="L19" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>117</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>118</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>121</v>
+        <v>147</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>122</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>123</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>124</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>125</v>
+        <v>151</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>128</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>129</v>
+        <v>155</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>130</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>131</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>132</v>
+        <v>158</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>133</v>
+        <v>159</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>135</v>
+        <v>161</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>136</v>
+        <v>162</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>137</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>139</v>
+        <v>165</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>140</v>
+        <v>166</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>141</v>
+        <v>167</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>142</v>
+        <v>168</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>143</v>
+        <v>169</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>144</v>
+        <v>170</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>145</v>
+        <v>171</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>146</v>
+        <v>172</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>147</v>
+        <v>173</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>148</v>
+        <v>174</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>149</v>
+        <v>175</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>150</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed a bug in the template generator's data validation, fills out xlsxfinalize
</commit_message>
<xml_diff>
--- a/bctw-api/src/import/test.xlsx
+++ b/bctw-api/src/import/test.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-26550" yWindow="2610" windowWidth="24765" windowHeight="14430"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28095" windowHeight="18240" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet sheetId="2" name="Device Metadata" state="visible" r:id="rId4"/>
-    <sheet sheetId="3" name="Validation" state="visible" r:id="rId5"/>
+    <sheet sheetId="4" name="Telemetry" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="Validation" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="187">
   <si>
     <t>Wildlife Health ID</t>
   </si>
@@ -56,7 +57,7 @@
     <t>Capture UTM Zone</t>
   </si>
   <si>
-    <t>Capture Comments</t>
+    <t>Capture Comment</t>
   </si>
   <si>
     <t>Ear Tag Right ID</t>
@@ -168,6 +169,36 @@
   </si>
   <si>
     <t>Mortality Comment</t>
+  </si>
+  <si>
+    <t>Device ID</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Acquisition Date</t>
+  </si>
+  <si>
+    <t>Elevation</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>Satellite</t>
+  </si>
+  <si>
+    <t>Dilution</t>
+  </si>
+  <si>
+    <t>Main Voltage</t>
+  </si>
+  <si>
+    <t>Backup Voltage</t>
   </si>
   <si>
     <t>Species Values</t>
@@ -1002,7 +1033,7 @@
   <dimension ref="A1:AY1"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="91" zoomScaleNormal="91">
-      <selection activeCell="AK4" sqref="AK4"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" defaultColWidth="10.7109375"/>
@@ -1174,40 +1205,40 @@
   </sheetData>
   <dataValidations count="12">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Selection" error="Please use the drop down to select a valid value" sqref="AD2:AD9999">
-      <formula1>Validation!F2:F4</formula1>
+      <formula1>Validation!$F$2:$F$4</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Selection" error="Please use the drop down to select a valid value" sqref="AE2:AE9999">
-      <formula1>Validation!G2:G7</formula1>
+      <formula1>Validation!$G$2:$G$7</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Selection" error="Please use the drop down to select a valid value" sqref="AG2:AG9999">
-      <formula1>Validation!H2:H5</formula1>
+      <formula1>Validation!$H$2:$H$5</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Selection" error="Please use the drop down to select a valid value" sqref="AI2:AI9999">
-      <formula1>Validation!I2:I4</formula1>
+      <formula1>Validation!$I$2:$I$4</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Selection" error="Please use the drop down to select a valid value" sqref="AL2:AL9999">
-      <formula1>Validation!J2:J4</formula1>
+      <formula1>Validation!$J$2:$J$4</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Selection" error="Please use the drop down to select a valid value" sqref="AT2:AT9999">
-      <formula1>Validation!K2:K8</formula1>
+      <formula1>Validation!$K$2:$K$8</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Selection" error="Please use the drop down to select a valid value" sqref="AX2:AX9999">
-      <formula1>Validation!L2:L19</formula1>
+      <formula1>Validation!$L$2:$L$19</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Selection" error="Please use the drop down to select a valid value" sqref="C2:C9999">
-      <formula1>Validation!A2:A5</formula1>
+      <formula1>Validation!$A$2:$A$5</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Selection" error="Please use the drop down to select a valid value" sqref="D2:D9999">
-      <formula1>Validation!B2:B56</formula1>
+      <formula1>Validation!$B$2:$B$56</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Selection" error="Please use the drop down to select a valid value" sqref="E2:E9999">
-      <formula1>Validation!C2:C10</formula1>
+      <formula1>Validation!$C$2:$C$10</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Selection" error="Please use the drop down to select a valid value" sqref="F2:F9999">
-      <formula1>Validation!D2:D4</formula1>
+      <formula1>Validation!$D$2:$D$4</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Selection" error="Please use the drop down to select a valid value" sqref="G2:G9999">
-      <formula1>Validation!E2:E6</formula1>
+      <formula1>Validation!$E$2:$E$6</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1225,513 +1256,577 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="E2" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="F2" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="G2" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="H2" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="I2" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="J2" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="K2" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="L2" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="D3" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="E3" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="F3" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G3" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="H3" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="I3" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="J3" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="K3" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="L3" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="C4" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="E4" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="F4" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="G4" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="H4" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="I4" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="J4" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="K4" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="L4" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="C5" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="E5" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="G5" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="H5" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="K5" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="L5" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="C6" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="E6" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="G6" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="K6" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="L6" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="C7" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="G7" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="K7" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="L7" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="C8" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="K8" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="L8" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="C9" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="L9" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="C10" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="L10" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="L11" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="L12" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="L13" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="L14" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="L15" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="L16" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="L17" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="L18" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="L19" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="45" customHeight="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+</worksheet>
 </file>
</xml_diff>